<commit_message>
new files - start working on master branch
</commit_message>
<xml_diff>
--- a/deeplearning1/excel/entropy_example.xlsx
+++ b/deeplearning1/excel/entropy_example.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27211"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j\Google Drive\Docs\fastai\course\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxwellmckinnon/dev/fastai/deeplearning1/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="21570" windowHeight="12900"/>
+    <workbookView xWindow="18560" yWindow="4360" windowWidth="32640" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="softmax" sheetId="2" r:id="rId1"/>
     <sheet name="entropy" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>isCat</t>
   </si>
@@ -55,12 +61,15 @@
   </si>
   <si>
     <t>building</t>
+  </si>
+  <si>
+    <t>softmax is an exponential weighting of the input to its other inputs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -436,100 +445,105 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2">
         <f ca="1">RAND()*10-5</f>
-        <v>-2.0756151098951037</v>
+        <v>-2.6644790538575283</v>
       </c>
       <c r="C2" s="2">
         <f ca="1">EXP(B2)</f>
-        <v>0.12547922024015928</v>
+        <v>6.96356204937571E-2</v>
       </c>
       <c r="D2" s="2">
         <f ca="1">C2/$C$7</f>
-        <v>1.3594323773306157E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>1.385894599859939E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:B6" ca="1" si="0">RAND()*10-5</f>
-        <v>-0.11171473940962784</v>
+        <f ca="1">RAND()*10-5</f>
+        <v>-2.1169792156246814</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C6" ca="1" si="1">EXP(B3)</f>
-        <v>0.89429932947233159</v>
+        <f t="shared" ref="C3:C6" ca="1" si="0">EXP(B3)</f>
+        <v>0.1203947663838735</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D6" ca="1" si="2">C3/$C$7</f>
-        <v>9.6887712657354658E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <f t="shared" ref="D3:D6" ca="1" si="1">C3/$C$7</f>
+        <v>2.3961078453773217E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2">
+        <f t="shared" ref="B3:B6" ca="1" si="2">RAND()*10-5</f>
+        <v>2.9288787323750887</v>
+      </c>
+      <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.269946142602584</v>
-      </c>
-      <c r="C4" s="2">
+        <v>18.706643579080119</v>
+      </c>
+      <c r="D4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5606607892681761</v>
-      </c>
-      <c r="D4" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.38575929563145001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.3723013614860512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>-2.6603243105950911</v>
+      </c>
+      <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.95184790801681629</v>
-      </c>
-      <c r="C5" s="2">
+        <v>6.9925540473322889E-2</v>
+      </c>
+      <c r="D5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38602702152495172</v>
-      </c>
-      <c r="D5" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.1821875413405561E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>1.391664614275302E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.4429588368640545</v>
+      </c>
+      <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4501606231001265</v>
-      </c>
-      <c r="C6" s="2">
+        <v>31.279371941032974</v>
+      </c>
+      <c r="D6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2637993248350918</v>
-      </c>
-      <c r="D6" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.4619367925244835</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0.6225249714544363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
       <c r="C7" s="2">
         <f ca="1">SUM(C2:C6)</f>
-        <v>9.2302656853407115</v>
+        <v>50.245971447464044</v>
       </c>
       <c r="D7" s="2">
         <f ca="1">SUM(D2:D6)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -541,13 +555,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>1</v>
       </c>
@@ -571,7 +585,7 @@
         <v>0.3010299956639812</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
@@ -587,7 +601,7 @@
         <v>8.7739243075051505E-3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>0</v>
       </c>
@@ -603,7 +617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>0</v>
       </c>
@@ -619,7 +633,7 @@
         <v>0.3010299956639812</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>1</v>
       </c>
@@ -635,7 +649,7 @@
         <v>4.5757490560675115E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C9">
         <f>25000*128*4/1000</f>
         <v>12800</v>

</xml_diff>